<commit_message>
lil' clean-up and added readme
</commit_message>
<xml_diff>
--- a/res/test.xlsx
+++ b/res/test.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aydar/Documents/PyCharmProjects/test_selenium_project/res/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0 ХД СКБ\Собеседования\Тест задания\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46DE53B-D446-024F-8920-D56A6CD87B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="14190" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="299">
   <si>
     <t>KindPremises</t>
   </si>
@@ -153,6 +152,18 @@
     <t xml:space="preserve">141892, Московская обл, Доронино, ул. , д. 0, </t>
   </si>
   <si>
+    <t>Чичерина</t>
+  </si>
+  <si>
+    <t>129327, Москва г, , ул. Чичерина, д. 2/9, кв. 233</t>
+  </si>
+  <si>
+    <t>Зеленоград</t>
+  </si>
+  <si>
+    <t>000000, Москва г, Зеленоград, ул. , д. 0, корп. 906, кв. 116</t>
+  </si>
+  <si>
     <t>Калининградская обл</t>
   </si>
   <si>
@@ -892,6 +903,15 @@
   </si>
   <si>
     <t>191002, Санкт-Петербург г, , ул. Реки Фонтанки, д. 50, кв. 51</t>
+  </si>
+  <si>
+    <t>Ковров</t>
+  </si>
+  <si>
+    <t>Сергея Лазо</t>
+  </si>
+  <si>
+    <t>601911, Владимирская обл, Ковров, ул. Сергея Лазо, д. 6/1, кв. 35</t>
   </si>
   <si>
     <t>Владимирская область</t>
@@ -906,7 +926,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -937,8 +957,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1218,29 +1239,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="97.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="97.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1275,7 +1296,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1304,7 +1325,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1336,7 +1357,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1362,7 +1383,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1391,7 +1412,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1420,7 +1441,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1452,7 +1473,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1475,65 +1496,62 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9">
-        <v>129594</v>
+        <v>129327</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" t="s">
-        <v>57</v>
+        <v>42</v>
+      </c>
+      <c r="H9" s="1">
+        <v>43345</v>
       </c>
       <c r="J9">
-        <v>59</v>
+        <v>233</v>
       </c>
       <c r="K9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>359450</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="H10">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>906</v>
       </c>
       <c r="J10">
-        <v>2</v>
+        <v>116</v>
       </c>
       <c r="K10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1541,19 +1559,19 @@
         <v>236001</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
         <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H11">
         <v>33</v>
@@ -1562,10 +1580,10 @@
         <v>12</v>
       </c>
       <c r="K11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1573,19 +1591,19 @@
         <v>309000</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F12" t="s">
         <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H12">
         <v>9</v>
@@ -1594,10 +1612,10 @@
         <v>4</v>
       </c>
       <c r="K12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1605,19 +1623,19 @@
         <v>170008</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
         <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H13">
         <v>70</v>
@@ -1629,721 +1647,724 @@
         <v>20</v>
       </c>
       <c r="K13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14">
-        <v>187556</v>
+        <v>129594</v>
       </c>
       <c r="C14" t="s">
-        <v>129</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" t="s">
-        <v>130</v>
+        <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>131</v>
-      </c>
-      <c r="G14">
+        <v>59</v>
+      </c>
+      <c r="G14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14">
+        <v>59</v>
+      </c>
+      <c r="K14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>359450</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15">
+        <v>9</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>196620</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="I16">
         <v>6</v>
       </c>
-      <c r="H14">
-        <v>10</v>
-      </c>
-      <c r="J14">
-        <v>119</v>
-      </c>
-      <c r="K14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B15">
-        <v>353320</v>
-      </c>
-      <c r="C15" t="s">
-        <v>94</v>
-      </c>
-      <c r="D15" t="s">
-        <v>219</v>
-      </c>
-      <c r="E15" t="s">
-        <v>242</v>
-      </c>
-      <c r="H15">
-        <v>223</v>
-      </c>
-      <c r="K15" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16">
-        <v>623428</v>
-      </c>
-      <c r="C16" t="s">
-        <v>177</v>
-      </c>
-      <c r="D16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" t="s">
-        <v>178</v>
-      </c>
-      <c r="F16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" t="s">
-        <v>277</v>
-      </c>
-      <c r="H16">
-        <v>48</v>
-      </c>
-      <c r="J16">
-        <v>32</v>
-      </c>
-      <c r="K16" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
       <c r="B17">
-        <v>196620</v>
+        <v>396341</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="F17" t="s">
         <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="H17">
-        <v>10</v>
-      </c>
-      <c r="I17">
-        <v>6</v>
-      </c>
-      <c r="J17">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="K17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
       <c r="B18">
-        <v>396341</v>
+        <v>142324</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" t="s">
-        <v>70</v>
-      </c>
-      <c r="H18">
-        <v>39</v>
+        <v>76</v>
+      </c>
+      <c r="H18" t="s">
+        <v>77</v>
       </c>
       <c r="K18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B19">
-        <v>142324</v>
+        <v>198302</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" t="s">
-        <v>72</v>
-      </c>
-      <c r="H19" t="s">
-        <v>73</v>
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" t="s">
+        <v>79</v>
+      </c>
+      <c r="H19">
+        <v>101</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>158</v>
       </c>
       <c r="K19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
       <c r="B20">
-        <v>198302</v>
+        <v>117534</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G20" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="H20">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="I20">
         <v>1</v>
       </c>
       <c r="J20">
-        <v>158</v>
+        <v>300</v>
       </c>
       <c r="K20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
       <c r="B21">
-        <v>117534</v>
+        <v>236019</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>46</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>47</v>
       </c>
       <c r="F21" t="s">
         <v>13</v>
       </c>
       <c r="G21" t="s">
-        <v>77</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
+        <v>83</v>
+      </c>
+      <c r="H21" t="s">
+        <v>84</v>
       </c>
       <c r="J21">
-        <v>300</v>
+        <v>20</v>
       </c>
       <c r="K21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
       <c r="B22">
-        <v>236019</v>
+        <v>396072</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
         <v>17</v>
       </c>
       <c r="E22" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="F22" t="s">
         <v>13</v>
       </c>
       <c r="G22" t="s">
-        <v>79</v>
-      </c>
-      <c r="H22" t="s">
-        <v>80</v>
+        <v>87</v>
+      </c>
+      <c r="H22">
+        <v>35</v>
+      </c>
+      <c r="I22" t="s">
+        <v>88</v>
       </c>
       <c r="J22">
         <v>20</v>
       </c>
       <c r="K22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
       <c r="B23">
-        <v>396072</v>
+        <v>198260</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="F23" t="s">
         <v>13</v>
       </c>
       <c r="G23" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="H23">
-        <v>35</v>
-      </c>
-      <c r="I23" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="J23">
-        <v>20</v>
+        <v>310</v>
       </c>
       <c r="K23" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
       <c r="B24">
-        <v>198260</v>
+        <v>117393</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F24" t="s">
         <v>13</v>
       </c>
       <c r="G24" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="H24">
-        <v>7</v>
+        <v>26</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
       </c>
       <c r="J24">
-        <v>310</v>
+        <v>635</v>
       </c>
       <c r="K24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
       <c r="B25">
-        <v>117393</v>
+        <v>777777</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" t="s">
+        <v>94</v>
       </c>
       <c r="F25" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="G25" t="s">
-        <v>88</v>
-      </c>
-      <c r="H25">
-        <v>26</v>
-      </c>
-      <c r="I25">
-        <v>3</v>
+        <v>95</v>
+      </c>
+      <c r="H25" t="s">
+        <v>96</v>
       </c>
       <c r="J25">
-        <v>635</v>
+        <v>22</v>
       </c>
       <c r="K25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
       <c r="B26">
-        <v>777777</v>
+        <v>354392</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E26" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="F26" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="G26" t="s">
-        <v>91</v>
-      </c>
-      <c r="H26" t="s">
-        <v>92</v>
+        <v>100</v>
+      </c>
+      <c r="H26">
+        <v>75</v>
       </c>
       <c r="J26">
         <v>22</v>
       </c>
       <c r="K26" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B27">
-        <v>354392</v>
+        <v>249192</v>
       </c>
       <c r="C27" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E27" t="s">
-        <v>95</v>
-      </c>
-      <c r="F27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="H27">
-        <v>75</v>
-      </c>
-      <c r="J27">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K27" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B28">
-        <v>249192</v>
+        <v>353900</v>
       </c>
       <c r="C28" t="s">
         <v>98</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>99</v>
+        <v>105</v>
+      </c>
+      <c r="F28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" t="s">
+        <v>106</v>
       </c>
       <c r="H28">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="K28" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>11</v>
       </c>
       <c r="B29">
-        <v>353900</v>
+        <v>353454</v>
       </c>
       <c r="C29" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D29" t="s">
         <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="F29" t="s">
         <v>13</v>
       </c>
       <c r="G29" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="H29">
+        <v>134</v>
+      </c>
+      <c r="J29">
+        <v>55</v>
+      </c>
+      <c r="K29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>346760</v>
+      </c>
+      <c r="C30" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" t="s">
+        <v>111</v>
+      </c>
+      <c r="F30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" t="s">
+        <v>112</v>
+      </c>
+      <c r="H30">
+        <v>18</v>
+      </c>
+      <c r="K30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31">
+        <v>169313</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" t="s">
+        <v>114</v>
+      </c>
+      <c r="F31" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" t="s">
+        <v>87</v>
+      </c>
+      <c r="H31">
+        <v>26</v>
+      </c>
+      <c r="J31">
+        <v>38</v>
+      </c>
+      <c r="K31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32">
+        <v>428020</v>
+      </c>
+      <c r="C32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" t="s">
+        <v>117</v>
+      </c>
+      <c r="F32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" t="s">
+        <v>118</v>
+      </c>
+      <c r="H32" t="s">
+        <v>119</v>
+      </c>
+      <c r="I32">
         <v>1</v>
       </c>
-      <c r="K29" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30">
-        <v>353454</v>
-      </c>
-      <c r="C30" t="s">
-        <v>94</v>
-      </c>
-      <c r="D30" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" t="s">
-        <v>104</v>
-      </c>
-      <c r="F30" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" t="s">
-        <v>36</v>
-      </c>
-      <c r="H30">
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33">
+        <v>350010</v>
+      </c>
+      <c r="C33" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" t="s">
+        <v>121</v>
+      </c>
+      <c r="F33" t="s">
+        <v>122</v>
+      </c>
+      <c r="G33" t="s">
+        <v>123</v>
+      </c>
+      <c r="H33">
+        <v>286</v>
+      </c>
+      <c r="K33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <v>117403</v>
+      </c>
+      <c r="C34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" t="s">
+        <v>59</v>
+      </c>
+      <c r="G34" t="s">
+        <v>125</v>
+      </c>
+      <c r="H34">
+        <v>14</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>43</v>
+      </c>
+      <c r="K34" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35">
+        <v>601966</v>
+      </c>
+      <c r="C35" t="s">
+        <v>127</v>
+      </c>
+      <c r="D35" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" t="s">
+        <v>128</v>
+      </c>
+      <c r="F35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" t="s">
+        <v>129</v>
+      </c>
+      <c r="H35">
+        <v>31</v>
+      </c>
+      <c r="K35" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36">
+        <v>198334</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" t="s">
+        <v>131</v>
+      </c>
+      <c r="H36">
+        <v>41</v>
+      </c>
+      <c r="J36">
+        <v>142</v>
+      </c>
+      <c r="K36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37">
+        <v>187556</v>
+      </c>
+      <c r="C37" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" t="s">
         <v>134</v>
       </c>
-      <c r="J30">
-        <v>55</v>
-      </c>
-      <c r="K30" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31">
-        <v>346760</v>
-      </c>
-      <c r="C31" t="s">
-        <v>106</v>
-      </c>
-      <c r="D31" t="s">
-        <v>68</v>
-      </c>
-      <c r="E31" t="s">
-        <v>107</v>
-      </c>
-      <c r="F31" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" t="s">
-        <v>108</v>
-      </c>
-      <c r="H31">
-        <v>18</v>
-      </c>
-      <c r="K31" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32">
-        <v>169313</v>
-      </c>
-      <c r="C32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" t="s">
-        <v>17</v>
-      </c>
-      <c r="E32" t="s">
-        <v>110</v>
-      </c>
-      <c r="F32" t="s">
-        <v>19</v>
-      </c>
-      <c r="G32" t="s">
-        <v>83</v>
-      </c>
-      <c r="H32">
-        <v>26</v>
-      </c>
-      <c r="J32">
-        <v>38</v>
-      </c>
-      <c r="K32" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33">
-        <v>428020</v>
-      </c>
-      <c r="C33" t="s">
-        <v>112</v>
-      </c>
-      <c r="D33" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" t="s">
-        <v>113</v>
-      </c>
-      <c r="F33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" t="s">
-        <v>114</v>
-      </c>
-      <c r="H33" t="s">
-        <v>115</v>
-      </c>
-      <c r="I33">
-        <v>1</v>
-      </c>
-      <c r="J33">
-        <v>1</v>
-      </c>
-      <c r="K33" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34">
-        <v>350010</v>
-      </c>
-      <c r="C34" t="s">
-        <v>94</v>
-      </c>
-      <c r="D34" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" t="s">
-        <v>117</v>
-      </c>
-      <c r="F34" t="s">
-        <v>118</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="F37" t="s">
+        <v>135</v>
+      </c>
+      <c r="G37">
+        <v>6</v>
+      </c>
+      <c r="H37">
+        <v>10</v>
+      </c>
+      <c r="J37">
         <v>119</v>
       </c>
-      <c r="H34">
-        <v>286</v>
-      </c>
-      <c r="K34" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B35">
-        <v>117403</v>
-      </c>
-      <c r="C35" t="s">
-        <v>25</v>
-      </c>
-      <c r="F35" t="s">
-        <v>55</v>
-      </c>
-      <c r="G35" t="s">
-        <v>121</v>
-      </c>
-      <c r="H35">
-        <v>14</v>
-      </c>
-      <c r="I35">
-        <v>1</v>
-      </c>
-      <c r="J35">
-        <v>43</v>
-      </c>
-      <c r="K35" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36">
-        <v>601966</v>
-      </c>
-      <c r="C36" t="s">
-        <v>123</v>
-      </c>
-      <c r="D36" t="s">
-        <v>60</v>
-      </c>
-      <c r="E36" t="s">
-        <v>124</v>
-      </c>
-      <c r="F36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" t="s">
-        <v>125</v>
-      </c>
-      <c r="H36">
-        <v>31</v>
-      </c>
-      <c r="K36" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37">
-        <v>198334</v>
-      </c>
-      <c r="C37" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" t="s">
-        <v>127</v>
-      </c>
-      <c r="H37">
-        <v>41</v>
-      </c>
-      <c r="J37">
-        <v>142</v>
-      </c>
       <c r="K37" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2357,7 +2378,7 @@
         <v>19</v>
       </c>
       <c r="G38" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="H38">
         <v>6</v>
@@ -2369,10 +2390,10 @@
         <v>519</v>
       </c>
       <c r="K38" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -2380,19 +2401,19 @@
         <v>188691</v>
       </c>
       <c r="C39" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D39" t="s">
         <v>39</v>
       </c>
       <c r="E39" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="F39" t="s">
         <v>13</v>
       </c>
       <c r="G39" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="H39">
         <v>11</v>
@@ -2404,10 +2425,10 @@
         <v>16</v>
       </c>
       <c r="K39" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -2415,19 +2436,19 @@
         <v>396039</v>
       </c>
       <c r="C40" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D40" t="s">
         <v>39</v>
       </c>
       <c r="E40" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="F40" t="s">
         <v>13</v>
       </c>
       <c r="G40" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H40">
         <v>2</v>
@@ -2436,10 +2457,10 @@
         <v>14</v>
       </c>
       <c r="K40" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -2447,28 +2468,28 @@
         <v>350915</v>
       </c>
       <c r="C41" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D41" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="E41" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F41" t="s">
         <v>13</v>
       </c>
       <c r="G41" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="H41">
         <v>83</v>
       </c>
       <c r="K41" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>29</v>
       </c>
@@ -2476,31 +2497,31 @@
         <v>353180</v>
       </c>
       <c r="C42" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D42" t="s">
         <v>17</v>
       </c>
       <c r="E42" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="F42" t="s">
         <v>13</v>
       </c>
       <c r="G42" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="H42">
         <v>12</v>
       </c>
       <c r="I42" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="K42" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -2508,19 +2529,19 @@
         <v>350040</v>
       </c>
       <c r="C43" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D43" t="s">
         <v>17</v>
       </c>
       <c r="E43" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F43" t="s">
         <v>13</v>
       </c>
       <c r="G43" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H43">
         <v>144</v>
@@ -2529,10 +2550,10 @@
         <v>30</v>
       </c>
       <c r="K43" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>29</v>
       </c>
@@ -2546,22 +2567,22 @@
         <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F44" t="s">
         <v>13</v>
       </c>
       <c r="G44" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H44" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="K44" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>29</v>
       </c>
@@ -2569,28 +2590,28 @@
         <v>618720</v>
       </c>
       <c r="C45" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D45" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E45" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="F45" t="s">
         <v>13</v>
       </c>
       <c r="G45" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="H45">
         <v>68</v>
       </c>
       <c r="K45" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -2598,19 +2619,19 @@
         <v>410062</v>
       </c>
       <c r="C46" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D46" t="s">
         <v>17</v>
       </c>
       <c r="E46" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="F46" t="s">
         <v>13</v>
       </c>
       <c r="G46" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="H46">
         <v>10</v>
@@ -2619,10 +2640,10 @@
         <v>132</v>
       </c>
       <c r="K46" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -2630,19 +2651,19 @@
         <v>353451</v>
       </c>
       <c r="C47" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D47" t="s">
         <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F47" t="s">
         <v>13</v>
       </c>
       <c r="G47" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="H47">
         <v>9</v>
@@ -2651,10 +2672,10 @@
         <v>67</v>
       </c>
       <c r="K47" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -2662,19 +2683,19 @@
         <v>236011</v>
       </c>
       <c r="C48" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D48" t="s">
         <v>17</v>
       </c>
       <c r="E48" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F48" t="s">
         <v>13</v>
       </c>
       <c r="G48" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="H48">
         <v>15</v>
@@ -2683,10 +2704,10 @@
         <v>4</v>
       </c>
       <c r="K48" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -2700,7 +2721,7 @@
         <v>13</v>
       </c>
       <c r="G49" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="H49">
         <v>4</v>
@@ -2709,10 +2730,10 @@
         <v>73</v>
       </c>
       <c r="K49" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>29</v>
       </c>
@@ -2720,28 +2741,28 @@
         <v>353217</v>
       </c>
       <c r="C50" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D50" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E50" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F50" t="s">
         <v>13</v>
       </c>
       <c r="G50" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H50">
         <v>5</v>
       </c>
       <c r="K50" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -2755,13 +2776,13 @@
         <v>17</v>
       </c>
       <c r="E51" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="F51" t="s">
         <v>13</v>
       </c>
       <c r="G51" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="H51">
         <v>108</v>
@@ -2770,10 +2791,10 @@
         <v>52</v>
       </c>
       <c r="K51" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>29</v>
       </c>
@@ -2781,28 +2802,28 @@
         <v>412913</v>
       </c>
       <c r="C52" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D52" t="s">
         <v>17</v>
       </c>
       <c r="E52" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="F52" t="s">
         <v>26</v>
       </c>
       <c r="G52" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="H52">
         <v>18</v>
       </c>
       <c r="K52" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>29</v>
       </c>
@@ -2810,28 +2831,28 @@
         <v>346760</v>
       </c>
       <c r="C53" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D53" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E53" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F53" t="s">
         <v>13</v>
       </c>
       <c r="G53" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="H53">
         <v>18</v>
       </c>
       <c r="K53" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>29</v>
       </c>
@@ -2839,22 +2860,22 @@
         <v>249192</v>
       </c>
       <c r="C54" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D54" t="s">
         <v>39</v>
       </c>
       <c r="E54" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="H54">
         <v>13</v>
       </c>
       <c r="K54" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>29</v>
       </c>
@@ -2862,28 +2883,28 @@
         <v>601966</v>
       </c>
       <c r="C55" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D55" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E55" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="F55" t="s">
         <v>13</v>
       </c>
       <c r="G55" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="H55">
         <v>31</v>
       </c>
       <c r="K55" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>11</v>
       </c>
@@ -2891,19 +2912,19 @@
         <v>623428</v>
       </c>
       <c r="C56" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D56" t="s">
         <v>17</v>
       </c>
       <c r="E56" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="F56" t="s">
         <v>13</v>
       </c>
       <c r="G56" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="H56">
         <v>16</v>
@@ -2912,10 +2933,10 @@
         <v>42</v>
       </c>
       <c r="K56" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>29</v>
       </c>
@@ -2923,28 +2944,28 @@
         <v>394008</v>
       </c>
       <c r="C57" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D57" t="s">
         <v>17</v>
       </c>
       <c r="E57" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="F57" t="s">
         <v>13</v>
       </c>
       <c r="G57" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="H57">
         <v>34</v>
       </c>
       <c r="K57" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>29</v>
       </c>
@@ -2952,28 +2973,28 @@
         <v>369012</v>
       </c>
       <c r="C58" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D58" t="s">
         <v>17</v>
       </c>
       <c r="E58" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="F58" t="s">
         <v>13</v>
       </c>
       <c r="G58" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="H58">
         <v>153</v>
       </c>
       <c r="K58" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>11</v>
       </c>
@@ -2987,13 +3008,13 @@
         <v>17</v>
       </c>
       <c r="E59" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="F59" t="s">
         <v>13</v>
       </c>
       <c r="G59" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="H59">
         <v>10</v>
@@ -3002,10 +3023,10 @@
         <v>250</v>
       </c>
       <c r="K59" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>29</v>
       </c>
@@ -3013,28 +3034,28 @@
         <v>352359</v>
       </c>
       <c r="C60" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D60" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E60" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="F60" t="s">
         <v>13</v>
       </c>
       <c r="G60" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="H60">
         <v>41</v>
       </c>
       <c r="K60" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>11</v>
       </c>
@@ -3042,19 +3063,19 @@
         <v>248033</v>
       </c>
       <c r="C61" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D61" t="s">
         <v>17</v>
       </c>
       <c r="E61" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="F61" t="s">
         <v>13</v>
       </c>
       <c r="G61" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="H61">
         <v>18</v>
@@ -3066,10 +3087,10 @@
         <v>164</v>
       </c>
       <c r="K61" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -3077,19 +3098,19 @@
         <v>173024</v>
       </c>
       <c r="C62" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D62" t="s">
         <v>17</v>
       </c>
       <c r="E62" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="F62" t="s">
         <v>19</v>
       </c>
       <c r="G62" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="H62">
         <v>47</v>
@@ -3098,10 +3119,10 @@
         <v>142</v>
       </c>
       <c r="K62" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -3109,19 +3130,19 @@
         <v>644117</v>
       </c>
       <c r="C63" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D63" t="s">
         <v>17</v>
       </c>
       <c r="E63" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="F63" t="s">
         <v>13</v>
       </c>
       <c r="G63" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="H63">
         <v>75</v>
@@ -3130,10 +3151,10 @@
         <v>179</v>
       </c>
       <c r="K63" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>29</v>
       </c>
@@ -3141,28 +3162,28 @@
         <v>346414</v>
       </c>
       <c r="C64" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D64" t="s">
         <v>17</v>
       </c>
       <c r="E64" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="F64" t="s">
         <v>13</v>
       </c>
       <c r="G64" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="H64" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="K64" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>29</v>
       </c>
@@ -3170,28 +3191,28 @@
         <v>350915</v>
       </c>
       <c r="C65" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D65" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="E65" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F65" t="s">
         <v>13</v>
       </c>
       <c r="G65" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="H65">
         <v>83</v>
       </c>
       <c r="K65" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>11</v>
       </c>
@@ -3199,19 +3220,19 @@
         <v>432030</v>
       </c>
       <c r="C66" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D66" t="s">
         <v>17</v>
       </c>
       <c r="E66" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="F66" t="s">
         <v>13</v>
       </c>
       <c r="G66" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="H66">
         <v>43</v>
@@ -3220,10 +3241,10 @@
         <v>13</v>
       </c>
       <c r="K66" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>29</v>
       </c>
@@ -3231,28 +3252,28 @@
         <v>601966</v>
       </c>
       <c r="C67" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D67" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E67" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="F67" t="s">
         <v>13</v>
       </c>
       <c r="G67" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="H67">
         <v>31</v>
       </c>
       <c r="K67" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>11</v>
       </c>
@@ -3260,19 +3281,19 @@
         <v>612960</v>
       </c>
       <c r="C68" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D68" t="s">
         <v>17</v>
       </c>
       <c r="E68" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="F68" t="s">
         <v>13</v>
       </c>
       <c r="G68" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="H68">
         <v>84</v>
@@ -3281,10 +3302,10 @@
         <v>37</v>
       </c>
       <c r="K68" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>29</v>
       </c>
@@ -3295,19 +3316,19 @@
         <v>38</v>
       </c>
       <c r="D69" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E69" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="H69">
         <v>475</v>
       </c>
       <c r="K69" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>29</v>
       </c>
@@ -3315,22 +3336,22 @@
         <v>160000</v>
       </c>
       <c r="C70" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="D70" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="E70" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="H70" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="K70" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>11</v>
       </c>
@@ -3338,19 +3359,19 @@
         <v>456910</v>
       </c>
       <c r="C71" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D71" t="s">
         <v>17</v>
       </c>
       <c r="E71" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="F71" t="s">
         <v>13</v>
       </c>
       <c r="G71" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="H71">
         <v>15</v>
@@ -3359,10 +3380,10 @@
         <v>11</v>
       </c>
       <c r="K71" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>11</v>
       </c>
@@ -3370,19 +3391,19 @@
         <v>214031</v>
       </c>
       <c r="C72" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D72" t="s">
         <v>17</v>
       </c>
       <c r="E72" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F72" t="s">
         <v>13</v>
       </c>
       <c r="G72" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="H72">
         <v>54</v>
@@ -3391,10 +3412,10 @@
         <v>10</v>
       </c>
       <c r="K72" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>11</v>
       </c>
@@ -3402,19 +3423,19 @@
         <v>236038</v>
       </c>
       <c r="C73" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D73" t="s">
         <v>17</v>
       </c>
       <c r="E73" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F73" t="s">
         <v>13</v>
       </c>
       <c r="G73" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="H73">
         <v>109</v>
@@ -3423,10 +3444,10 @@
         <v>40</v>
       </c>
       <c r="K73" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>11</v>
       </c>
@@ -3434,19 +3455,19 @@
         <v>644117</v>
       </c>
       <c r="C74" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D74" t="s">
         <v>17</v>
       </c>
       <c r="E74" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="F74" t="s">
         <v>13</v>
       </c>
       <c r="G74" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="H74">
         <v>75</v>
@@ -3455,10 +3476,10 @@
         <v>179</v>
       </c>
       <c r="K74" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>11</v>
       </c>
@@ -3472,13 +3493,13 @@
         <v>17</v>
       </c>
       <c r="E75" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="F75" t="s">
         <v>13</v>
       </c>
       <c r="G75" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="H75">
         <v>10</v>
@@ -3487,10 +3508,10 @@
         <v>250</v>
       </c>
       <c r="K75" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>11</v>
       </c>
@@ -3501,16 +3522,16 @@
         <v>38</v>
       </c>
       <c r="D76" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="E76" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F76" t="s">
         <v>13</v>
       </c>
       <c r="G76" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="H76">
         <v>5</v>
@@ -3519,10 +3540,10 @@
         <v>20</v>
       </c>
       <c r="K76" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>11</v>
       </c>
@@ -3530,31 +3551,31 @@
         <v>305001</v>
       </c>
       <c r="C77" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="D77" t="s">
         <v>17</v>
       </c>
       <c r="E77" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="F77" t="s">
         <v>13</v>
       </c>
       <c r="G77" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="H77" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="J77">
         <v>17</v>
       </c>
       <c r="K77" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>29</v>
       </c>
@@ -3562,22 +3583,22 @@
         <v>353320</v>
       </c>
       <c r="C78" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D78" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="E78" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="H78">
         <v>223</v>
       </c>
       <c r="K78" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>29</v>
       </c>
@@ -3585,28 +3606,28 @@
         <v>644013</v>
       </c>
       <c r="C79" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D79" t="s">
         <v>17</v>
       </c>
       <c r="E79" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="F79" t="s">
         <v>13</v>
       </c>
       <c r="G79" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="H79">
         <v>7</v>
       </c>
       <c r="K79" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>11</v>
       </c>
@@ -3614,13 +3635,13 @@
         <v>777777</v>
       </c>
       <c r="C80" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="E80" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G80" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="H80">
         <v>31</v>
@@ -3629,10 +3650,10 @@
         <v>58</v>
       </c>
       <c r="K80" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>11</v>
       </c>
@@ -3643,16 +3664,16 @@
         <v>38</v>
       </c>
       <c r="D81" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E81" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F81" t="s">
         <v>13</v>
       </c>
       <c r="G81" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="H81">
         <v>2</v>
@@ -3661,10 +3682,10 @@
         <v>48</v>
       </c>
       <c r="K81" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -3672,19 +3693,19 @@
         <v>454071</v>
       </c>
       <c r="C82" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D82" t="s">
         <v>17</v>
       </c>
       <c r="E82" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="F82" t="s">
         <v>13</v>
       </c>
       <c r="G82" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="H82">
         <v>3</v>
@@ -3693,10 +3714,10 @@
         <v>10</v>
       </c>
       <c r="K82" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>11</v>
       </c>
@@ -3704,28 +3725,28 @@
         <v>462218</v>
       </c>
       <c r="C83" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="D83" t="s">
         <v>39</v>
       </c>
       <c r="E83" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="F83" t="s">
         <v>13</v>
       </c>
       <c r="G83" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="H83">
         <v>61</v>
       </c>
       <c r="K83" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>29</v>
       </c>
@@ -3733,28 +3754,28 @@
         <v>456560</v>
       </c>
       <c r="C84" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D84" t="s">
         <v>31</v>
       </c>
       <c r="E84" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="F84" t="s">
         <v>26</v>
       </c>
       <c r="G84" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="H84">
         <v>5</v>
       </c>
       <c r="K84" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>29</v>
       </c>
@@ -3762,28 +3783,28 @@
         <v>413044</v>
       </c>
       <c r="C85" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D85" t="s">
         <v>31</v>
       </c>
       <c r="E85" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="F85" t="s">
         <v>13</v>
       </c>
       <c r="G85" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="H85" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="K85" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>29</v>
       </c>
@@ -3791,28 +3812,28 @@
         <v>456871</v>
       </c>
       <c r="C86" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D86" t="s">
         <v>17</v>
       </c>
       <c r="E86" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="F86" t="s">
         <v>13</v>
       </c>
       <c r="G86" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="H86">
         <v>230</v>
       </c>
       <c r="K86" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>29</v>
       </c>
@@ -3820,28 +3841,28 @@
         <v>601966</v>
       </c>
       <c r="C87" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D87" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E87" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="F87" t="s">
         <v>13</v>
       </c>
       <c r="G87" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="H87">
         <v>31</v>
       </c>
       <c r="K87" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>11</v>
       </c>
@@ -3849,19 +3870,19 @@
         <v>644117</v>
       </c>
       <c r="C88" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D88" t="s">
         <v>17</v>
       </c>
       <c r="E88" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="F88" t="s">
         <v>13</v>
       </c>
       <c r="G88" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="H88">
         <v>75</v>
@@ -3870,10 +3891,10 @@
         <v>179</v>
       </c>
       <c r="K88" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>29</v>
       </c>
@@ -3881,28 +3902,28 @@
         <v>305019</v>
       </c>
       <c r="C89" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="D89" t="s">
         <v>17</v>
       </c>
       <c r="E89" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="F89" t="s">
         <v>13</v>
       </c>
       <c r="G89" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="H89">
         <v>50</v>
       </c>
       <c r="K89" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>11</v>
       </c>
@@ -3910,19 +3931,19 @@
         <v>453252</v>
       </c>
       <c r="C90" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="D90" t="s">
         <v>17</v>
       </c>
       <c r="E90" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="F90" t="s">
         <v>13</v>
       </c>
       <c r="G90" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="H90">
         <v>3</v>
@@ -3931,10 +3952,10 @@
         <v>32</v>
       </c>
       <c r="K90" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>11</v>
       </c>
@@ -3948,7 +3969,7 @@
         <v>19</v>
       </c>
       <c r="G91" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="H91">
         <v>159</v>
@@ -3960,10 +3981,10 @@
         <v>15</v>
       </c>
       <c r="K91" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>11</v>
       </c>
@@ -3971,19 +3992,19 @@
         <v>454100</v>
       </c>
       <c r="C92" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D92" t="s">
         <v>17</v>
       </c>
       <c r="E92" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="F92" t="s">
         <v>13</v>
       </c>
       <c r="G92" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="H92">
         <v>3</v>
@@ -3992,82 +4013,73 @@
         <v>164</v>
       </c>
       <c r="K92" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B93">
-        <v>119034</v>
+        <v>353320</v>
       </c>
       <c r="C93" t="s">
-        <v>25</v>
-      </c>
-      <c r="F93" t="s">
-        <v>26</v>
-      </c>
-      <c r="G93" t="s">
-        <v>279</v>
+        <v>98</v>
+      </c>
+      <c r="D93" t="s">
+        <v>223</v>
+      </c>
+      <c r="E93" t="s">
+        <v>246</v>
       </c>
       <c r="H93">
-        <v>5</v>
-      </c>
-      <c r="J93">
-        <v>18</v>
+        <v>223</v>
       </c>
       <c r="K93" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>11</v>
       </c>
       <c r="B94">
-        <v>644010</v>
+        <v>623428</v>
       </c>
       <c r="C94" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="D94" t="s">
         <v>17</v>
       </c>
       <c r="E94" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="F94" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G94" t="s">
         <v>281</v>
       </c>
       <c r="H94">
-        <v>119</v>
+        <v>48</v>
       </c>
       <c r="J94">
-        <v>141</v>
+        <v>32</v>
       </c>
       <c r="K94" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>11</v>
       </c>
       <c r="B95">
-        <v>454077</v>
+        <v>119034</v>
       </c>
       <c r="C95" t="s">
-        <v>223</v>
-      </c>
-      <c r="D95" t="s">
-        <v>17</v>
-      </c>
-      <c r="E95" t="s">
-        <v>250</v>
+        <v>25</v>
       </c>
       <c r="F95" t="s">
         <v>26</v>
@@ -4076,100 +4088,196 @@
         <v>283</v>
       </c>
       <c r="H95">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J95">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="K95" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B96">
-        <v>413044</v>
+        <v>644010</v>
       </c>
       <c r="C96" t="s">
-        <v>158</v>
+        <v>205</v>
       </c>
       <c r="D96" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E96" t="s">
-        <v>260</v>
+        <v>206</v>
       </c>
       <c r="F96" t="s">
         <v>13</v>
       </c>
       <c r="G96" t="s">
-        <v>261</v>
+        <v>285</v>
       </c>
       <c r="H96">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="J96">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="K96" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>11</v>
       </c>
       <c r="B97">
-        <v>191002</v>
+        <v>454077</v>
       </c>
       <c r="C97" t="s">
-        <v>12</v>
+        <v>227</v>
+      </c>
+      <c r="D97" t="s">
+        <v>17</v>
+      </c>
+      <c r="E97" t="s">
+        <v>254</v>
       </c>
       <c r="F97" t="s">
-        <v>286</v>
+        <v>26</v>
       </c>
       <c r="G97" t="s">
         <v>287</v>
       </c>
       <c r="H97">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="J97">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="K97" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>29</v>
       </c>
       <c r="B98">
+        <v>413044</v>
+      </c>
+      <c r="C98" t="s">
+        <v>162</v>
+      </c>
+      <c r="D98" t="s">
+        <v>31</v>
+      </c>
+      <c r="E98" t="s">
+        <v>264</v>
+      </c>
+      <c r="F98" t="s">
+        <v>13</v>
+      </c>
+      <c r="G98" t="s">
+        <v>265</v>
+      </c>
+      <c r="H98">
+        <v>90</v>
+      </c>
+      <c r="J98">
+        <v>2</v>
+      </c>
+      <c r="K98" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>11</v>
+      </c>
+      <c r="B99">
+        <v>191002</v>
+      </c>
+      <c r="C99" t="s">
+        <v>12</v>
+      </c>
+      <c r="F99" t="s">
+        <v>290</v>
+      </c>
+      <c r="G99" t="s">
+        <v>291</v>
+      </c>
+      <c r="H99">
+        <v>50</v>
+      </c>
+      <c r="J99">
+        <v>51</v>
+      </c>
+      <c r="K99" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>11</v>
+      </c>
+      <c r="B100">
+        <v>601911</v>
+      </c>
+      <c r="C100" t="s">
+        <v>127</v>
+      </c>
+      <c r="D100" t="s">
+        <v>17</v>
+      </c>
+      <c r="E100" t="s">
+        <v>293</v>
+      </c>
+      <c r="F100" t="s">
+        <v>13</v>
+      </c>
+      <c r="G100" t="s">
+        <v>294</v>
+      </c>
+      <c r="H100" s="1">
+        <v>43106</v>
+      </c>
+      <c r="J100">
+        <v>35</v>
+      </c>
+      <c r="K100" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>29</v>
+      </c>
+      <c r="B101">
         <v>601966</v>
       </c>
-      <c r="C98" t="s">
-        <v>289</v>
-      </c>
-      <c r="D98" t="s">
-        <v>290</v>
-      </c>
-      <c r="E98" t="s">
-        <v>124</v>
-      </c>
-      <c r="F98" t="s">
-        <v>13</v>
-      </c>
-      <c r="G98" t="s">
-        <v>125</v>
-      </c>
-      <c r="H98">
+      <c r="C101" t="s">
+        <v>296</v>
+      </c>
+      <c r="D101" t="s">
+        <v>297</v>
+      </c>
+      <c r="E101" t="s">
+        <v>128</v>
+      </c>
+      <c r="F101" t="s">
+        <v>13</v>
+      </c>
+      <c r="G101" t="s">
+        <v>129</v>
+      </c>
+      <c r="H101">
         <v>31</v>
       </c>
-      <c r="K98" t="s">
-        <v>291</v>
+      <c r="K101" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>